<commit_message>
april update 2 - figures
</commit_message>
<xml_diff>
--- a/correlations/ttest_results.xlsx
+++ b/correlations/ttest_results.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Programozás\rsa-hub-and-spokes\correlations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68808A6E-F260-4E9E-9D28-A42E09955C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45D84A7-BB65-451D-87DD-56061BC0D3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ttest" sheetId="1" r:id="rId1"/>
-    <sheet name="ttest_cond" sheetId="2" r:id="rId2"/>
+    <sheet name="ttest_cond" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>ROI</t>
   </si>
@@ -145,37 +144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -483,252 +452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2">
-        <v>1.9131816795142671</v>
-      </c>
-      <c r="D2">
-        <v>6.1577309450291828E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.105561101914786</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <v>3.185741485470428</v>
-      </c>
-      <c r="D3">
-        <v>2.5124170810792799E-3</v>
-      </c>
-      <c r="E3">
-        <v>1.5074502486475679E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>2.282373368939973</v>
-      </c>
-      <c r="D4">
-        <v>2.684609015205993E-2</v>
-      </c>
-      <c r="E4">
-        <v>7.8795582955210511E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>3.7713010983173332</v>
-      </c>
-      <c r="D5">
-        <v>4.3786540414756948E-4</v>
-      </c>
-      <c r="E5">
-        <v>5.2543848497708344E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>0.82952301512970117</v>
-      </c>
-      <c r="D6">
-        <v>0.41083155697532048</v>
-      </c>
-      <c r="E6">
-        <v>0.44817988033671319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7">
-        <v>2.4712237625870941</v>
-      </c>
-      <c r="D7">
-        <v>1.698940104759479E-2</v>
-      </c>
-      <c r="E7">
-        <v>6.7957604190379148E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-      <c r="C8">
-        <v>2.1165871247002919</v>
-      </c>
-      <c r="D8">
-        <v>3.9397791477605262E-2</v>
-      </c>
-      <c r="E8">
-        <v>7.8795582955210511E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>50</v>
-      </c>
-      <c r="C9">
-        <v>0.73193326938167103</v>
-      </c>
-      <c r="D9">
-        <v>0.46769572075160037</v>
-      </c>
-      <c r="E9">
-        <v>0.46769572075160037</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10">
-        <v>1.0225961369726331</v>
-      </c>
-      <c r="D10">
-        <v>0.31152108883628621</v>
-      </c>
-      <c r="E10">
-        <v>0.41536145178171502</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>2.1820574997484972</v>
-      </c>
-      <c r="D11">
-        <v>3.3929692229053503E-2</v>
-      </c>
-      <c r="E11">
-        <v>7.8795582955210511E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>1.792912038503347</v>
-      </c>
-      <c r="D12">
-        <v>7.916069238424879E-2</v>
-      </c>
-      <c r="E12">
-        <v>0.11874103857637321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>0.87128844312193177</v>
-      </c>
-      <c r="D13">
-        <v>0.38784568034617151</v>
-      </c>
-      <c r="E13">
-        <v>0.44817988033671319</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1234,13 +962,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="E1:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>